<commit_message>
sheet 2 = all data points, not just avg
</commit_message>
<xml_diff>
--- a/data-raw/growth_rates_summary_wip.xlsx
+++ b/data-raw/growth_rates_summary_wip.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\Documents\B Lab\cross-tolerance\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115D345B-BDC9-4135-944C-DF51863DAA2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1574C256-1653-4970-B07C-4F7EC55EECDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{311CE9AC-D601-4DF3-8159-B4D668D6C29C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{311CE9AC-D601-4DF3-8159-B4D668D6C29C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,19 +37,109 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>avg actual temp</t>
   </si>
   <si>
     <t>avg growth rate</t>
+  </si>
+  <si>
+    <t>temp</t>
+  </si>
+  <si>
+    <t>growth rate</t>
+  </si>
+  <si>
+    <t>6.978653 </t>
+  </si>
+  <si>
+    <t>7.13187 </t>
+  </si>
+  <si>
+    <t>5.427084 </t>
+  </si>
+  <si>
+    <t>7.139992 </t>
+  </si>
+  <si>
+    <t>7.023783 </t>
+  </si>
+  <si>
+    <t>7.258182 </t>
+  </si>
+  <si>
+    <t>7.156545 </t>
+  </si>
+  <si>
+    <t>8.051096 </t>
+  </si>
+  <si>
+    <t>8.119615 </t>
+  </si>
+  <si>
+    <t>11.44259 </t>
+  </si>
+  <si>
+    <t>10.72757 </t>
+  </si>
+  <si>
+    <t>10.68343 </t>
+  </si>
+  <si>
+    <t>11.225 </t>
+  </si>
+  <si>
+    <t>10.61753 </t>
+  </si>
+  <si>
+    <t>6.7881 </t>
+  </si>
+  <si>
+    <t>6.373724 </t>
+  </si>
+  <si>
+    <t>3.125253 </t>
+  </si>
+  <si>
+    <t>3.972342 </t>
+  </si>
+  <si>
+    <t>3.28597 </t>
+  </si>
+  <si>
+    <t>6.06593 </t>
+  </si>
+  <si>
+    <t>7.904557 </t>
+  </si>
+  <si>
+    <t>2.772583 </t>
+  </si>
+  <si>
+    <t>2.677185 </t>
+  </si>
+  <si>
+    <t>2.568138 </t>
+  </si>
+  <si>
+    <t>2.593191 </t>
+  </si>
+  <si>
+    <t>1.970546 </t>
+  </si>
+  <si>
+    <t>2.75412 </t>
+  </si>
+  <si>
+    <t>2.607848 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +165,12 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF444746"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -111,7 +208,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -123,6 +220,8 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA800000-642D-497B-8059-A61ADE3033CB}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,34 +586,666 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
-        <v>40.04607</v>
-      </c>
-      <c r="B6" s="3">
-        <v>8.2861910000000005</v>
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9.0005459999999999</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
-        <v>40.116849999999999</v>
+        <v>40.535420000000002</v>
       </c>
       <c r="B7" s="2">
-        <v>9.0005459999999999</v>
+        <v>5.7611970000000001</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.50291</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C40890-5FB8-4C42-A3AD-60610C49A445}">
+  <dimension ref="A1:B81"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="B81" sqref="B81"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.1003318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>18</v>
+      </c>
+      <c r="B3" s="5">
+        <v>9.9472569999999996E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>18</v>
+      </c>
+      <c r="B4" s="5">
+        <v>9.9491609999999994E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>18</v>
+      </c>
+      <c r="B5" s="5">
+        <v>9.8961060000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>18</v>
+      </c>
+      <c r="B6" s="5">
+        <v>0.10189860000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>18</v>
+      </c>
+      <c r="B7" s="5">
+        <v>9.7996799999999995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>18</v>
+      </c>
+      <c r="B8" s="5">
+        <v>9.7644229999999999E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <v>0.10099859999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B17" s="5">
+        <v>7.0355239999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B18" s="5">
+        <v>8.8879839999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B19" s="5">
+        <v>9.1432889999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B20" s="5">
+        <v>8.8955749999999991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B21" s="5">
+        <v>9.0471590000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B22" s="5">
+        <v>9.0021679999999993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B23" s="5">
+        <v>8.9892319999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B24" s="5">
+        <v>10.67995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B25" s="5">
+        <v>8.9228000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B26" s="5">
+        <v>8.9139230000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B27" s="5">
+        <v>9.0081030000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B28" s="5">
+        <v>8.7893570000000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B29" s="5">
+        <v>8.7185349999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B37" s="5">
+        <v>8.0467929999999992</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B38" s="5">
+        <v>10.187290000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B39" s="5">
+        <v>7.463965</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B40" s="5">
+        <v>9.7239989999999992</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B41" s="5">
+        <v>5.4158989999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B42" s="5">
+        <v>10.54608</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B43" s="5">
+        <v>7.5910469999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B44" s="5">
+        <v>10.436120000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B45" s="5">
+        <v>10.63997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
         <v>40.535420000000002</v>
       </c>
-      <c r="B8" s="2">
-        <v>5.7611970000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="B46" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B53" s="5">
+        <v>8.5736969999999992</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
         <v>41.180900000000001</v>
       </c>
-      <c r="B9" s="3">
-        <v>1.50291</v>
+      <c r="B54" s="5">
+        <v>1.248718</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B55" s="5">
+        <v>8.7624300000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B56" s="5">
+        <v>0.76345470000000004</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B57" s="5">
+        <v>0.5987903</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B58" s="5">
+        <v>0.4896916</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B59" s="5">
+        <v>0.48276409999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B60" s="5">
+        <v>0.48143750000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B61" s="5">
+        <v>0.50883769999999995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B62" s="5">
+        <v>0.86194800000000005</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B63" s="5">
+        <v>1.178188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B64" s="5">
+        <v>1.075391</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="2">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B65" s="5">
+        <v>1.583267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="6">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="6">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="6">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="6">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="6">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="6">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="6">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="6">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B73" s="5">
+        <v>2.4336829999999998</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="6">
+        <v>42.059730000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="6">
+        <v>42.059730000000002</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="6">
+        <v>42.059730000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="6">
+        <v>42.059730000000002</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="6">
+        <v>42.059730000000002</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="6">
+        <v>42.059730000000002</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="6">
+        <v>42.059730000000002</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="6">
+        <v>42.059730000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
no more white spaces
</commit_message>
<xml_diff>
--- a/data-raw/growth_rates_summary_wip.xlsx
+++ b/data-raw/growth_rates_summary_wip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\Documents\B Lab\cross-tolerance\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513134BF-E6AA-49A1-AFAA-7FC6A172F40E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6CC649-0F0A-4646-AD6F-B0C033C96AD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{311CE9AC-D601-4DF3-8159-B4D668D6C29C}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>avg actual temp</t>
   </si>
@@ -72,90 +72,6 @@
   </si>
   <si>
     <t>growth rate</t>
-  </si>
-  <si>
-    <t>6.978653 </t>
-  </si>
-  <si>
-    <t>7.13187 </t>
-  </si>
-  <si>
-    <t>5.427084 </t>
-  </si>
-  <si>
-    <t>7.139992 </t>
-  </si>
-  <si>
-    <t>7.023783 </t>
-  </si>
-  <si>
-    <t>7.258182 </t>
-  </si>
-  <si>
-    <t>7.156545 </t>
-  </si>
-  <si>
-    <t>8.051096 </t>
-  </si>
-  <si>
-    <t>8.119615 </t>
-  </si>
-  <si>
-    <t>11.44259 </t>
-  </si>
-  <si>
-    <t>10.72757 </t>
-  </si>
-  <si>
-    <t>10.68343 </t>
-  </si>
-  <si>
-    <t>11.225 </t>
-  </si>
-  <si>
-    <t>10.61753 </t>
-  </si>
-  <si>
-    <t>6.7881 </t>
-  </si>
-  <si>
-    <t>6.373724 </t>
-  </si>
-  <si>
-    <t>3.125253 </t>
-  </si>
-  <si>
-    <t>3.972342 </t>
-  </si>
-  <si>
-    <t>3.28597 </t>
-  </si>
-  <si>
-    <t>6.06593 </t>
-  </si>
-  <si>
-    <t>7.904557 </t>
-  </si>
-  <si>
-    <t>2.772583 </t>
-  </si>
-  <si>
-    <t>2.677185 </t>
-  </si>
-  <si>
-    <t>2.568138 </t>
-  </si>
-  <si>
-    <t>2.593191 </t>
-  </si>
-  <si>
-    <t>1.970546 </t>
-  </si>
-  <si>
-    <t>2.75412 </t>
-  </si>
-  <si>
-    <t>2.607848 </t>
   </si>
   <si>
     <t>avg temp</t>
@@ -190,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0000000"/>
+    <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -279,12 +195,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -682,7 +598,7 @@
   <dimension ref="A1:B81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A81" sqref="A81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,56 +682,56 @@
       <c r="A10" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>4</v>
+      <c r="B10" s="6">
+        <v>6.9786530000000004</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>5</v>
+      <c r="B11" s="6">
+        <v>7.1318700000000002</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>6</v>
+      <c r="B12" s="6">
+        <v>5.4270839999999998</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>7</v>
+      <c r="B13" s="6">
+        <v>7.1399920000000003</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>8</v>
+      <c r="B14" s="6">
+        <v>7.0237829999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>9</v>
+      <c r="B15" s="6">
+        <v>7.2581819999999997</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>10</v>
+      <c r="B16" s="6">
+        <v>7.1565450000000004</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -926,56 +842,56 @@
       <c r="A30" s="7">
         <v>37.310420000000001</v>
       </c>
-      <c r="B30" s="6" t="s">
-        <v>11</v>
+      <c r="B30" s="6">
+        <v>8.0510959999999994</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="7">
         <v>37.310420000000001</v>
       </c>
-      <c r="B31" s="6" t="s">
-        <v>12</v>
+      <c r="B31" s="6">
+        <v>8.1196149999999996</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="7">
         <v>37.310420000000001</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>13</v>
+      <c r="B32" s="6">
+        <v>11.442589999999999</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="7">
         <v>37.310420000000001</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>14</v>
+      <c r="B33" s="6">
+        <v>10.72757</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="7">
         <v>37.310420000000001</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>15</v>
+      <c r="B34" s="6">
+        <v>10.68343</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>37.310420000000001</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>16</v>
+      <c r="B35" s="6">
+        <v>11.225</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="7">
         <v>37.310420000000001</v>
       </c>
-      <c r="B36" s="6" t="s">
-        <v>17</v>
+      <c r="B36" s="6">
+        <v>10.61753</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1054,56 +970,56 @@
       <c r="A46" s="7">
         <v>40.535420000000002</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>18</v>
+      <c r="B46" s="6">
+        <v>6.7881</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
         <v>40.535420000000002</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>19</v>
+      <c r="B47" s="6">
+        <v>6.3737240000000002</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
         <v>40.535420000000002</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>20</v>
+      <c r="B48" s="6">
+        <v>3.1252529999999998</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>40.535420000000002</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>21</v>
+      <c r="B49" s="6">
+        <v>3.9723419999999998</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
         <v>40.535420000000002</v>
       </c>
-      <c r="B50" s="6" t="s">
-        <v>22</v>
+      <c r="B50" s="6">
+        <v>3.2859699999999998</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
         <v>40.535420000000002</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>23</v>
+      <c r="B51" s="6">
+        <v>6.0659299999999998</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>40.535420000000002</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>24</v>
+      <c r="B52" s="6">
+        <v>7.9045569999999996</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1214,56 +1130,56 @@
       <c r="A66" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B66" s="6" t="s">
-        <v>25</v>
+      <c r="B66" s="6">
+        <v>2.772583</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>26</v>
+      <c r="B67" s="6">
+        <v>2.6771850000000001</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B68" s="6" t="s">
-        <v>27</v>
+      <c r="B68" s="6">
+        <v>2.5681379999999998</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B69" s="6" t="s">
-        <v>28</v>
+      <c r="B69" s="6">
+        <v>2.593191</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B70" s="6" t="s">
-        <v>29</v>
+      <c r="B70" s="6">
+        <v>1.9705459999999999</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B71" s="6" t="s">
-        <v>30</v>
+      <c r="B71" s="6">
+        <v>2.7541199999999999</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B72" s="6" t="s">
-        <v>31</v>
+      <c r="B72" s="6">
+        <v>2.6078480000000002</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -1275,51 +1191,35 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
-        <v>42.059730000000002</v>
-      </c>
+      <c r="A74" s="8"/>
       <c r="B74" s="5"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="8">
-        <v>42.059730000000002</v>
-      </c>
+      <c r="A75" s="8"/>
       <c r="B75" s="5"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
-        <v>42.059730000000002</v>
-      </c>
+      <c r="A76" s="8"/>
       <c r="B76" s="5"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="8">
-        <v>42.059730000000002</v>
-      </c>
+      <c r="A77" s="8"/>
       <c r="B77" s="5"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
-        <v>42.059730000000002</v>
-      </c>
+      <c r="A78" s="8"/>
       <c r="B78" s="5"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="8">
-        <v>42.059730000000002</v>
-      </c>
+      <c r="A79" s="8"/>
       <c r="B79" s="5"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="8">
-        <v>42.059730000000002</v>
-      </c>
+      <c r="A80" s="8"/>
       <c r="B80" s="5"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="8">
-        <v>42.059730000000002</v>
-      </c>
+      <c r="A81" s="8"/>
       <c r="B81" s="5"/>
     </row>
   </sheetData>
@@ -1340,31 +1240,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="G1" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
-        <v>39</v>
+        <v>11</v>
       </c>
       <c r="I1" t="s">
-        <v>40</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1401,27 +1301,27 @@
       <c r="A3" s="2">
         <v>25.367419999999999</v>
       </c>
-      <c r="B3" t="str" cm="1">
+      <c r="B3" cm="1">
         <f t="array" ref="B3:I3">TRANSPOSE(Sheet2!B10:B17)</f>
-        <v>6.978653 </v>
-      </c>
-      <c r="C3" t="str">
-        <v>7.13187 </v>
-      </c>
-      <c r="D3" t="str">
-        <v>5.427084 </v>
-      </c>
-      <c r="E3" t="str">
-        <v>7.139992 </v>
-      </c>
-      <c r="F3" t="str">
-        <v>7.023783 </v>
-      </c>
-      <c r="G3" t="str">
-        <v>7.258182 </v>
-      </c>
-      <c r="H3" t="str">
-        <v>7.156545 </v>
+        <v>6.9786530000000004</v>
+      </c>
+      <c r="C3">
+        <v>7.1318700000000002</v>
+      </c>
+      <c r="D3">
+        <v>5.4270839999999998</v>
+      </c>
+      <c r="E3">
+        <v>7.1399920000000003</v>
+      </c>
+      <c r="F3">
+        <v>7.0237829999999999</v>
+      </c>
+      <c r="G3">
+        <v>7.2581819999999997</v>
+      </c>
+      <c r="H3">
+        <v>7.1565450000000004</v>
       </c>
       <c r="I3">
         <v>7.0355239999999997</v>

</xml_diff>

<commit_message>
sheet 2 = both 41 deg data, sheet 3 = 24hr 41 deg, sheet 4 = 48 hr 41 deg
</commit_message>
<xml_diff>
--- a/data-raw/growth_rates_summary_wip.xlsx
+++ b/data-raw/growth_rates_summary_wip.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\Documents\B Lab\cross-tolerance\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3EC297-2ABB-4D56-B52F-41B5CFB82F98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40026439-2A6B-4D6F-B00C-817F021CA6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{311CE9AC-D601-4DF3-8159-B4D668D6C29C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{311CE9AC-D601-4DF3-8159-B4D668D6C29C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="41_deg_from_june_30" sheetId="4" r:id="rId3"/>
+    <sheet name="41_deg_from_july_13" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,30 +38,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>avg actual temp</t>
   </si>
@@ -73,33 +52,6 @@
   <si>
     <t>growth rate</t>
   </si>
-  <si>
-    <t>avg temp</t>
-  </si>
-  <si>
-    <t>growth rate 1</t>
-  </si>
-  <si>
-    <t>growth rate 2</t>
-  </si>
-  <si>
-    <t>growth rate 3</t>
-  </si>
-  <si>
-    <t>growth rate 4</t>
-  </si>
-  <si>
-    <t>growth rate 5</t>
-  </si>
-  <si>
-    <t>growth rate 6</t>
-  </si>
-  <si>
-    <t>growth rate 7</t>
-  </si>
-  <si>
-    <t>growth rate 8</t>
-  </si>
 </sst>
 </file>
 
@@ -108,7 +60,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -142,10 +94,16 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="8"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -156,7 +114,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -179,11 +137,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -203,6 +191,22 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -597,10 +601,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C40890-5FB8-4C42-A3AD-60610C49A445}">
-  <dimension ref="A1:B81"/>
+  <dimension ref="A1:D81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="D79" sqref="D79"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,15 +612,16 @@
     <col min="1" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D1" s="15"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>18</v>
       </c>
@@ -624,7 +629,7 @@
         <v>0.1003318</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>18</v>
       </c>
@@ -632,7 +637,7 @@
         <v>9.9472569999999996E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>18</v>
       </c>
@@ -640,7 +645,7 @@
         <v>9.9491609999999994E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>18</v>
       </c>
@@ -648,7 +653,7 @@
         <v>9.8961060000000003E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>18</v>
       </c>
@@ -656,7 +661,7 @@
         <v>0.10189860000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>18</v>
       </c>
@@ -664,7 +669,7 @@
         <v>9.7996799999999995E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>18</v>
       </c>
@@ -672,7 +677,7 @@
         <v>9.7644229999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>18</v>
       </c>
@@ -680,7 +685,7 @@
         <v>0.10099859999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>25.367419999999999</v>
       </c>
@@ -688,7 +693,7 @@
         <v>6.9786530000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>25.367419999999999</v>
       </c>
@@ -696,7 +701,7 @@
         <v>7.1318700000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="7">
         <v>25.367419999999999</v>
       </c>
@@ -704,7 +709,7 @@
         <v>5.4270839999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7">
         <v>25.367419999999999</v>
       </c>
@@ -712,7 +717,7 @@
         <v>7.1399920000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>25.367419999999999</v>
       </c>
@@ -720,7 +725,7 @@
         <v>7.0237829999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>25.367419999999999</v>
       </c>
@@ -728,7 +733,7 @@
         <v>7.2581819999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <v>25.367419999999999</v>
       </c>
@@ -1263,106 +1268,1170 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEA6DFD0-88DD-43F0-A662-3BCED9AD47B2}">
-  <dimension ref="A1:I3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B9AB1CC-11C1-4860-B226-EBB6A9821896}">
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
         <v>18</v>
       </c>
-      <c r="B2" cm="1">
-        <f t="array" ref="B2:I2">TRANSPOSE(Sheet2!B2:B9)</f>
+      <c r="B2" s="12">
         <v>0.1003318</v>
       </c>
-      <c r="C2">
-        <v>9.9472569999999996E-2</v>
-      </c>
-      <c r="D2">
-        <v>9.9491609999999994E-2</v>
-      </c>
-      <c r="E2">
-        <v>9.8961060000000003E-2</v>
-      </c>
-      <c r="F2">
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>18</v>
+      </c>
+      <c r="B3" s="12">
+        <v>9.9472599999999994E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>18</v>
+      </c>
+      <c r="B4" s="12">
+        <v>9.9491599999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>18</v>
+      </c>
+      <c r="B5" s="12">
+        <v>9.8961099999999996E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>18</v>
+      </c>
+      <c r="B6" s="12">
         <v>0.10189860000000001</v>
       </c>
-      <c r="G2">
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>18</v>
+      </c>
+      <c r="B7" s="12">
         <v>9.7996799999999995E-2</v>
       </c>
-      <c r="H2">
-        <v>9.7644229999999999E-2</v>
-      </c>
-      <c r="I2">
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>18</v>
+      </c>
+      <c r="B8" s="12">
+        <v>9.76442E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>18</v>
+      </c>
+      <c r="B9" s="12">
         <v>0.10099859999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B3" cm="1">
-        <f t="array" ref="B3:I3">TRANSPOSE(Sheet2!B10:B17)</f>
+      <c r="B10" s="12">
         <v>6.9786530000000004</v>
       </c>
-      <c r="C3">
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B11" s="12">
         <v>7.1318700000000002</v>
       </c>
-      <c r="D3">
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B12" s="12">
         <v>5.4270839999999998</v>
       </c>
-      <c r="E3">
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B13" s="12">
         <v>7.1399920000000003</v>
       </c>
-      <c r="F3">
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B14" s="12">
         <v>7.0237829999999999</v>
       </c>
-      <c r="G3">
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B15" s="12">
         <v>7.2581819999999997</v>
       </c>
-      <c r="H3">
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B16" s="12">
         <v>7.1565450000000004</v>
       </c>
-      <c r="I3">
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B17" s="12">
         <v>7.0355239999999997</v>
       </c>
     </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B18" s="12">
+        <v>8.8879839999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B19" s="12">
+        <v>9.1432889999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B20" s="12">
+        <v>8.8955749999999991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B21" s="12">
+        <v>9.0471590000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B22" s="12">
+        <v>9.0021679999999993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B23" s="12">
+        <v>8.9892319999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B24" s="12">
+        <v>10.67995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B25" s="12">
+        <v>8.9228000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B26" s="12">
+        <v>8.9139230000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B27" s="12">
+        <v>9.0081030000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B28" s="12">
+        <v>8.7893570000000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B29" s="12">
+        <v>8.7185349999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B30" s="12">
+        <v>8.0510959999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B31" s="12">
+        <v>8.1196149999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B32" s="12">
+        <v>11.442589999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B33" s="12">
+        <v>10.72757</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B34" s="12">
+        <v>10.68343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B35" s="12">
+        <v>11.225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B36" s="12">
+        <v>10.61753</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B37" s="12">
+        <v>8.0467929999999992</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B38" s="12">
+        <v>10.187290000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B39" s="12">
+        <v>7.463965</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B40" s="12">
+        <v>9.7239989999999992</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B41" s="12">
+        <v>5.4158989999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B42" s="12">
+        <v>10.54608</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B43" s="12">
+        <v>7.5910469999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B44" s="12">
+        <v>10.436120000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B45" s="12">
+        <v>10.63997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B46" s="12">
+        <v>6.7881</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B47" s="12">
+        <v>6.3737240000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B48" s="12">
+        <v>3.1252529999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B49" s="12">
+        <v>3.9723419999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B50" s="12">
+        <v>3.2859699999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B51" s="12">
+        <v>6.0659299999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B52" s="12">
+        <v>7.9045569999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B53" s="12">
+        <v>8.5736969999999992</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="13">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B54" s="12">
+        <v>1.248718</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B55" s="12">
+        <v>8.7624300000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B56" s="12">
+        <v>0.76345470000000004</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B57" s="12">
+        <v>0.5987903</v>
+      </c>
+      <c r="D57" s="15">
+        <v>45107</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B58" s="12">
+        <v>0.4896916</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B59" s="12">
+        <v>0.48276409999999997</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B60" s="12">
+        <v>0.48143750000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B61" s="12">
+        <v>0.50883769999999995</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B62" s="12">
+        <v>0.86194800000000005</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B63" s="12">
+        <v>1.178188</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B64" s="12">
+        <v>1.075391</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="14">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B65" s="12">
+        <v>1.583267</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B66" s="12">
+        <v>0.83187169999999999</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B67" s="12">
+        <v>0.57295079999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B68" s="12">
+        <v>1.7377849999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B69" s="12">
+        <v>1.593799</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B70" s="12">
+        <v>1.0861190000000001</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B71" s="12">
+        <v>0.96393479999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B72" s="12">
+        <v>1.6751320000000001</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B73" s="12">
+        <v>3.156685</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF1A63C-18D1-4235-B644-4B61D0A0FCC0}">
+  <dimension ref="A1:B69"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="11">
+        <v>18</v>
+      </c>
+      <c r="B2" s="12">
+        <v>0.1003318</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>18</v>
+      </c>
+      <c r="B3" s="12">
+        <v>9.9472599999999994E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11">
+        <v>18</v>
+      </c>
+      <c r="B4" s="12">
+        <v>9.9491599999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11">
+        <v>18</v>
+      </c>
+      <c r="B5" s="12">
+        <v>9.8961099999999996E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11">
+        <v>18</v>
+      </c>
+      <c r="B6" s="12">
+        <v>0.10189860000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11">
+        <v>18</v>
+      </c>
+      <c r="B7" s="12">
+        <v>9.7996799999999995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="11">
+        <v>18</v>
+      </c>
+      <c r="B8" s="12">
+        <v>9.76442E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11">
+        <v>18</v>
+      </c>
+      <c r="B9" s="12">
+        <v>0.10099859999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="13">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B10" s="12">
+        <v>6.9786530000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B11" s="12">
+        <v>7.1318700000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B12" s="12">
+        <v>5.4270839999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B13" s="12">
+        <v>7.1399920000000003</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B14" s="12">
+        <v>7.0237829999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B15" s="12">
+        <v>7.2581819999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B16" s="12">
+        <v>7.1565450000000004</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="14">
+        <v>25.367419999999999</v>
+      </c>
+      <c r="B17" s="12">
+        <v>7.0355239999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B18" s="12">
+        <v>8.8879839999999994</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B19" s="12">
+        <v>9.1432889999999993</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B20" s="12">
+        <v>8.8955749999999991</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B21" s="12">
+        <v>9.0471590000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B22" s="12">
+        <v>9.0021679999999993</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B23" s="12">
+        <v>8.9892319999999994</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B24" s="12">
+        <v>10.67995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B25" s="12">
+        <v>8.9228000000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B26" s="12">
+        <v>8.9139230000000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B27" s="12">
+        <v>9.0081030000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B28" s="12">
+        <v>8.7893570000000008</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B29" s="12">
+        <v>8.7185349999999993</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="13">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B30" s="12">
+        <v>8.0510959999999994</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B31" s="12">
+        <v>8.1196149999999996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B32" s="12">
+        <v>11.442589999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B33" s="12">
+        <v>10.72757</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B34" s="12">
+        <v>10.68343</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B35" s="12">
+        <v>11.225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B36" s="12">
+        <v>10.61753</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="14">
+        <v>37.310420000000001</v>
+      </c>
+      <c r="B37" s="12">
+        <v>8.0467929999999992</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B38" s="12">
+        <v>10.187290000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B39" s="12">
+        <v>7.463965</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B40" s="12">
+        <v>9.7239989999999992</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B41" s="12">
+        <v>5.4158989999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B42" s="12">
+        <v>10.54608</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B43" s="12">
+        <v>7.5910469999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B44" s="12">
+        <v>10.436120000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B45" s="12">
+        <v>10.63997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B46" s="12">
+        <v>6.7881</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B47" s="12">
+        <v>6.3737240000000002</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B48" s="12">
+        <v>3.1252529999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B49" s="12">
+        <v>3.9723419999999998</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B50" s="12">
+        <v>3.2859699999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B51" s="12">
+        <v>6.0659299999999998</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B52" s="12">
+        <v>7.9045569999999996</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B53" s="12">
+        <v>8.5736969999999992</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="16">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B54" s="12">
+        <v>2.772583</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="16">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B55" s="12">
+        <v>2.6771850000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="16">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B56" s="12">
+        <v>2.5681379999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="16">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B57" s="12">
+        <v>2.593191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="16">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B58" s="12">
+        <v>1.9705459999999999</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="16">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B59" s="12">
+        <v>2.7541199999999999</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="16">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B60" s="12">
+        <v>2.6078480000000002</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="16">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B61" s="12">
+        <v>2.4336829999999998</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B62" s="12">
+        <v>0.83187169999999999</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B63" s="12">
+        <v>0.57295079999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B64" s="12">
+        <v>1.7377849999999999</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B65" s="12">
+        <v>1.593799</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B66" s="12">
+        <v>1.0861190000000001</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B67" s="12">
+        <v>0.96393479999999998</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B68" s="12">
+        <v>1.6751320000000001</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B69" s="12">
+        <v>3.156685</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added july 25, 30 deg
</commit_message>
<xml_diff>
--- a/data-raw/growth_rates_summary_wip.xlsx
+++ b/data-raw/growth_rates_summary_wip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\Documents\B Lab\cross-tolerance\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40026439-2A6B-4D6F-B00C-817F021CA6A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74B5478-9C4F-437D-8FF0-51B202F6ECF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{311CE9AC-D601-4DF3-8159-B4D668D6C29C}"/>
   </bookViews>
@@ -171,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -206,6 +206,9 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1871,10 +1874,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDF1A63C-18D1-4235-B644-4B61D0A0FCC0}">
-  <dimension ref="A1:B69"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2015,76 +2018,76 @@
         <v>7.0355239999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B18" s="12">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>30.255669999999999</v>
+      </c>
+      <c r="B18">
+        <v>6.7203929999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>30.255669999999999</v>
+      </c>
+      <c r="B19">
+        <v>9.1037090000000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>30.255669999999999</v>
+      </c>
+      <c r="B20">
+        <v>9.2296230000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>30.255669999999999</v>
+      </c>
+      <c r="B21">
+        <v>9.0925360000000008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>30.255669999999999</v>
+      </c>
+      <c r="B22">
+        <v>9.1172039999999992</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>30.255669999999999</v>
+      </c>
+      <c r="B23">
+        <v>8.9201910000000009</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>30.255669999999999</v>
+      </c>
+      <c r="B24">
+        <v>9.0851369999999996</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="17">
+        <v>30.255669999999999</v>
+      </c>
+      <c r="B25">
+        <v>6.7645799999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B26" s="12">
         <v>8.8879839999999994</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B19" s="12">
-        <v>9.1432889999999993</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B20" s="12">
-        <v>8.8955749999999991</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B21" s="12">
-        <v>9.0471590000000006</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B22" s="12">
-        <v>9.0021679999999993</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B23" s="12">
-        <v>8.9892319999999994</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B24" s="12">
-        <v>10.67995</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B25" s="12">
-        <v>8.9228000000000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B26" s="12">
-        <v>8.9139230000000005</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2092,7 +2095,7 @@
         <v>34.135959999999997</v>
       </c>
       <c r="B27" s="12">
-        <v>9.0081030000000002</v>
+        <v>9.1432889999999993</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2100,7 +2103,7 @@
         <v>34.135959999999997</v>
       </c>
       <c r="B28" s="12">
-        <v>8.7893570000000008</v>
+        <v>8.8955749999999991</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2108,330 +2111,395 @@
         <v>34.135959999999997</v>
       </c>
       <c r="B29" s="12">
-        <v>8.7185349999999993</v>
+        <v>9.0471590000000006</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13">
-        <v>37.310420000000001</v>
+      <c r="A30" s="14">
+        <v>34.135959999999997</v>
       </c>
       <c r="B30" s="12">
-        <v>8.0510959999999994</v>
+        <v>9.0021679999999993</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="14">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B31" s="12">
-        <v>8.1196149999999996</v>
+        <v>8.9892319999999994</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="14">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B32" s="12">
-        <v>11.442589999999999</v>
+        <v>10.67995</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="14">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B33" s="12">
-        <v>10.72757</v>
+        <v>8.9228000000000005</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="14">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B34" s="12">
-        <v>10.68343</v>
+        <v>8.9139230000000005</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="14">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B35" s="12">
-        <v>11.225</v>
+        <v>9.0081030000000002</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="14">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B36" s="12">
-        <v>10.61753</v>
+        <v>8.7893570000000008</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B37" s="12">
+        <v>8.7185349999999993</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B37" s="12">
-        <v>8.0467929999999992</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14">
-        <v>40.116849999999999</v>
-      </c>
       <c r="B38" s="12">
-        <v>10.187290000000001</v>
+        <v>8.0510959999999994</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="14">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B39" s="12">
-        <v>7.463965</v>
+        <v>8.1196149999999996</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="14">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B40" s="12">
-        <v>9.7239989999999992</v>
+        <v>11.442589999999999</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="14">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B41" s="12">
-        <v>5.4158989999999996</v>
+        <v>10.72757</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="14">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B42" s="12">
-        <v>10.54608</v>
+        <v>10.68343</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="14">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B43" s="12">
-        <v>7.5910469999999997</v>
+        <v>11.225</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="14">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B44" s="12">
-        <v>10.436120000000001</v>
+        <v>10.61753</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="14">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B45" s="12">
-        <v>10.63997</v>
+        <v>8.0467929999999992</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="14">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B46" s="12">
-        <v>6.7881</v>
+        <v>10.187290000000001</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="14">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B47" s="12">
-        <v>6.3737240000000002</v>
+        <v>7.463965</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="14">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B48" s="12">
-        <v>3.1252529999999998</v>
+        <v>9.7239989999999992</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="14">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B49" s="12">
-        <v>3.9723419999999998</v>
+        <v>5.4158989999999996</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="14">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B50" s="12">
-        <v>3.2859699999999998</v>
+        <v>10.54608</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B51" s="12">
-        <v>6.0659299999999998</v>
+        <v>7.5910469999999997</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="14">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B52" s="12">
-        <v>7.9045569999999996</v>
+        <v>10.436120000000001</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="14">
+        <v>40.116849999999999</v>
+      </c>
+      <c r="B53" s="12">
+        <v>10.63997</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="14">
         <v>40.535420000000002</v>
       </c>
-      <c r="B53" s="12">
+      <c r="B54" s="12">
+        <v>6.7881</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B55" s="12">
+        <v>6.3737240000000002</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B56" s="12">
+        <v>3.1252529999999998</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B57" s="12">
+        <v>3.9723419999999998</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B58" s="12">
+        <v>3.2859699999999998</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B59" s="12">
+        <v>6.0659299999999998</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B60" s="12">
+        <v>7.9045569999999996</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="14">
+        <v>40.535420000000002</v>
+      </c>
+      <c r="B61" s="12">
         <v>8.5736969999999992</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="16">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B54" s="12">
-        <v>2.772583</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B55" s="12">
-        <v>2.6771850000000001</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="16">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B56" s="12">
-        <v>2.5681379999999998</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="16">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B57" s="12">
-        <v>2.593191</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="16">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B58" s="12">
-        <v>1.9705459999999999</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="16">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B59" s="12">
-        <v>2.7541199999999999</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="16">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B60" s="12">
-        <v>2.6078480000000002</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="16">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B61" s="12">
-        <v>2.4336829999999998</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16">
-        <v>42.059730000000002</v>
+        <v>40.980829999999997</v>
       </c>
       <c r="B62" s="12">
-        <v>0.83187169999999999</v>
+        <v>2.772583</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16">
-        <v>42.059730000000002</v>
+        <v>40.980829999999997</v>
       </c>
       <c r="B63" s="12">
-        <v>0.57295079999999998</v>
+        <v>2.6771850000000001</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="16">
-        <v>42.059730000000002</v>
+        <v>40.980829999999997</v>
       </c>
       <c r="B64" s="12">
-        <v>1.7377849999999999</v>
+        <v>2.5681379999999998</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="16">
-        <v>42.059730000000002</v>
+        <v>40.980829999999997</v>
       </c>
       <c r="B65" s="12">
-        <v>1.593799</v>
+        <v>2.593191</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="16">
-        <v>42.059730000000002</v>
+        <v>40.980829999999997</v>
       </c>
       <c r="B66" s="12">
-        <v>1.0861190000000001</v>
+        <v>1.9705459999999999</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="16">
-        <v>42.059730000000002</v>
+        <v>40.980829999999997</v>
       </c>
       <c r="B67" s="12">
-        <v>0.96393479999999998</v>
+        <v>2.7541199999999999</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="16">
-        <v>42.059730000000002</v>
+        <v>40.980829999999997</v>
       </c>
       <c r="B68" s="12">
-        <v>1.6751320000000001</v>
+        <v>2.6078480000000002</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="16">
+        <v>40.980829999999997</v>
+      </c>
+      <c r="B69" s="12">
+        <v>2.4336829999999998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="16">
         <v>42.059730000000002</v>
       </c>
-      <c r="B69" s="12">
+      <c r="B70" s="12">
+        <v>0.83187169999999999</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B71" s="12">
+        <v>0.57295079999999998</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B72" s="12">
+        <v>1.7377849999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B73" s="12">
+        <v>1.593799</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B74" s="12">
+        <v>1.0861190000000001</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B75" s="12">
+        <v>0.96393479999999998</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B76" s="12">
+        <v>1.6751320000000001</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="16">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B77" s="12">
         <v>3.156685</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added july 25 20 deg
</commit_message>
<xml_diff>
--- a/data-raw/growth_rates_summary_wip.xlsx
+++ b/data-raw/growth_rates_summary_wip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\Documents\B Lab\cross-tolerance\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75688116-B747-4CBA-BC60-3A94E0E4B6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D059B9-5DF1-4584-926B-0D0B68AE5135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{311CE9AC-D601-4DF3-8159-B4D668D6C29C}"/>
   </bookViews>
@@ -604,10 +604,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C40890-5FB8-4C42-A3AD-60610C49A445}">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,7 +680,7 @@
         <v>9.7644229999999999E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>18</v>
       </c>
@@ -688,196 +688,196 @@
         <v>0.10099859999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>2.5196809999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>2.5673010000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>2.5868950000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>2.4982829999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>2.577801</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>20</v>
+      </c>
+      <c r="B15">
+        <v>2.5949309999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>2.5599249999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>2.5691769999999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B18" s="6">
         <v>6.9786530000000004</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="7">
+    <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B11" s="6">
+      <c r="B19" s="6">
         <v>7.1318700000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
+    <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B12" s="6">
+      <c r="B20" s="6">
         <v>5.4270839999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
+    <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B21" s="6">
         <v>7.1399920000000003</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7">
+    <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B22" s="6">
         <v>7.0237829999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7">
+    <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B23" s="6">
         <v>7.2581819999999997</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
+    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B16" s="6">
+      <c r="B24" s="6">
         <v>7.1565450000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
         <v>25.367419999999999</v>
       </c>
-      <c r="B17" s="6">
+      <c r="B25" s="6">
         <v>7.0355239999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" s="17">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
         <v>30.255669999999999</v>
       </c>
-      <c r="B18">
+      <c r="B26">
         <v>6.7203929999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="17">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
         <v>30.255669999999999</v>
       </c>
-      <c r="B19">
+      <c r="B27">
         <v>9.1037090000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
         <v>30.255669999999999</v>
       </c>
-      <c r="B20">
+      <c r="B28">
         <v>9.2296230000000001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="17">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
         <v>30.255669999999999</v>
       </c>
-      <c r="B21">
+      <c r="B29">
         <v>9.0925360000000008</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="17">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
         <v>30.255669999999999</v>
       </c>
-      <c r="B22">
+      <c r="B30">
         <v>9.1172039999999992</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="17">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="17">
         <v>30.255669999999999</v>
       </c>
-      <c r="B23">
+      <c r="B31">
         <v>8.9201910000000009</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="17">
         <v>30.255669999999999</v>
       </c>
-      <c r="B24">
+      <c r="B32">
         <v>9.0851369999999996</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="17">
+    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="17">
         <v>30.255669999999999</v>
       </c>
-      <c r="B25">
+      <c r="B33">
         <v>6.7645799999999996</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="7">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B26" s="6">
-        <v>8.8879839999999994</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="7">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B27" s="6">
-        <v>9.1432889999999993</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B28" s="6">
-        <v>8.8955749999999991</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="7">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B29" s="6">
-        <v>9.0471590000000006</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="7">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B30" s="6">
-        <v>9.0021679999999993</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="7">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B31" s="6">
-        <v>8.9892319999999994</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="7">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B32" s="6">
-        <v>10.67995</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="7">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B33" s="6">
-        <v>8.9228000000000005</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -885,7 +885,7 @@
         <v>34.135959999999997</v>
       </c>
       <c r="B34" s="6">
-        <v>8.9139230000000005</v>
+        <v>8.8879839999999994</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -893,7 +893,7 @@
         <v>34.135959999999997</v>
       </c>
       <c r="B35" s="6">
-        <v>9.0081030000000002</v>
+        <v>9.1432889999999993</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -901,7 +901,7 @@
         <v>34.135959999999997</v>
       </c>
       <c r="B36" s="6">
-        <v>8.7893570000000008</v>
+        <v>8.8955749999999991</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -909,263 +909,263 @@
         <v>34.135959999999997</v>
       </c>
       <c r="B37" s="6">
-        <v>8.7185349999999993</v>
+        <v>9.0471590000000006</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="7">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B38" s="6">
-        <v>8.0510959999999994</v>
+        <v>9.0021679999999993</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="7">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B39" s="6">
-        <v>8.1196149999999996</v>
+        <v>8.9892319999999994</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="7">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B40" s="6">
-        <v>11.442589999999999</v>
+        <v>10.67995</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="7">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B41" s="6">
-        <v>10.72757</v>
+        <v>8.9228000000000005</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B42" s="6">
-        <v>10.68343</v>
+        <v>8.9139230000000005</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="7">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B43" s="6">
-        <v>11.225</v>
+        <v>9.0081030000000002</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="7">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B44" s="6">
-        <v>10.61753</v>
+        <v>8.7893570000000008</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="7">
-        <v>37.310420000000001</v>
+        <v>34.135959999999997</v>
       </c>
       <c r="B45" s="6">
-        <v>8.0467929999999992</v>
+        <v>8.7185349999999993</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B46" s="6">
-        <v>10.187290000000001</v>
+        <v>8.0510959999999994</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="7">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B47" s="6">
-        <v>7.463965</v>
+        <v>8.1196149999999996</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="7">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B48" s="6">
-        <v>9.7239989999999992</v>
+        <v>11.442589999999999</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B49" s="6">
-        <v>5.4158989999999996</v>
+        <v>10.72757</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="7">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B50" s="6">
-        <v>10.54608</v>
+        <v>10.68343</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="7">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B51" s="6">
-        <v>7.5910469999999997</v>
+        <v>11.225</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B52" s="6">
-        <v>10.436120000000001</v>
+        <v>10.61753</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="7">
-        <v>40.116849999999999</v>
+        <v>37.310420000000001</v>
       </c>
       <c r="B53" s="6">
-        <v>10.63997</v>
+        <v>8.0467929999999992</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="7">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B54" s="6">
-        <v>6.7881</v>
+        <v>10.187290000000001</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B55" s="6">
-        <v>6.3737240000000002</v>
+        <v>7.463965</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="7">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B56" s="6">
-        <v>3.1252529999999998</v>
+        <v>9.7239989999999992</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B57" s="6">
-        <v>3.9723419999999998</v>
+        <v>5.4158989999999996</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="7">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B58" s="6">
-        <v>3.2859699999999998</v>
+        <v>10.54608</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B59" s="6">
-        <v>6.0659299999999998</v>
+        <v>7.5910469999999997</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="7">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B60" s="6">
-        <v>7.9045569999999996</v>
+        <v>10.436120000000001</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="7">
-        <v>40.535420000000002</v>
+        <v>40.116849999999999</v>
       </c>
       <c r="B61" s="6">
-        <v>8.5736969999999992</v>
+        <v>10.63997</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="7">
-        <v>41.180900000000001</v>
+        <v>40.535420000000002</v>
       </c>
       <c r="B62" s="6">
-        <v>1.248718</v>
+        <v>6.7881</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="7">
-        <v>41.180900000000001</v>
+        <v>40.535420000000002</v>
       </c>
       <c r="B63" s="6">
-        <v>8.7624300000000002</v>
+        <v>6.3737240000000002</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="7">
-        <v>41.180900000000001</v>
+        <v>40.535420000000002</v>
       </c>
       <c r="B64" s="6">
-        <v>0.76345470000000004</v>
+        <v>3.1252529999999998</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="7">
-        <v>41.180900000000001</v>
+        <v>40.535420000000002</v>
       </c>
       <c r="B65" s="6">
-        <v>0.5987903</v>
+        <v>3.9723419999999998</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="7">
-        <v>41.180900000000001</v>
+        <v>40.535420000000002</v>
       </c>
       <c r="B66" s="6">
-        <v>0.4896916</v>
+        <v>3.2859699999999998</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="7">
-        <v>41.180900000000001</v>
+        <v>40.535420000000002</v>
       </c>
       <c r="B67" s="6">
-        <v>0.48276409999999997</v>
+        <v>6.0659299999999998</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="7">
-        <v>41.180900000000001</v>
+        <v>40.535420000000002</v>
       </c>
       <c r="B68" s="6">
-        <v>0.48143750000000002</v>
+        <v>7.9045569999999996</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="7">
-        <v>41.180900000000001</v>
+        <v>40.535420000000002</v>
       </c>
       <c r="B69" s="6">
-        <v>0.50883769999999995</v>
+        <v>8.5736969999999992</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1173,7 +1173,7 @@
         <v>41.180900000000001</v>
       </c>
       <c r="B70" s="6">
-        <v>0.86194800000000005</v>
+        <v>1.248718</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1181,7 +1181,7 @@
         <v>41.180900000000001</v>
       </c>
       <c r="B71" s="6">
-        <v>1.178188</v>
+        <v>8.7624300000000002</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1189,7 +1189,7 @@
         <v>41.180900000000001</v>
       </c>
       <c r="B72" s="6">
-        <v>1.075391</v>
+        <v>0.76345470000000004</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1197,134 +1197,198 @@
         <v>41.180900000000001</v>
       </c>
       <c r="B73" s="6">
+        <v>0.5987903</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="7">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B74" s="6">
+        <v>0.4896916</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="7">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B75" s="6">
+        <v>0.48276409999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="7">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B76" s="6">
+        <v>0.48143750000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="7">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B77" s="6">
+        <v>0.50883769999999995</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="7">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B78" s="6">
+        <v>0.86194800000000005</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="7">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B79" s="6">
+        <v>1.178188</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="7">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B80" s="6">
+        <v>1.075391</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="7">
+        <v>41.180900000000001</v>
+      </c>
+      <c r="B81" s="6">
         <v>1.583267</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="8">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B74" s="6">
+      <c r="B82" s="6">
         <v>2.772583</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="8">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B75" s="6">
+      <c r="B83" s="6">
         <v>2.6771850000000001</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="8">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B76" s="6">
+      <c r="B84" s="6">
         <v>2.5681379999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="8">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B77" s="6">
+      <c r="B85" s="6">
         <v>2.593191</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="8">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B78" s="6">
+      <c r="B86" s="6">
         <v>1.9705459999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="8">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B79" s="6">
+      <c r="B87" s="6">
         <v>2.7541199999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="8">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B80" s="6">
+      <c r="B88" s="6">
         <v>2.6078480000000002</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="8">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="8">
         <v>40.980829999999997</v>
       </c>
-      <c r="B81" s="6">
+      <c r="B89" s="6">
         <v>2.4336829999999998</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="10">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="10">
         <v>42.059730000000002</v>
       </c>
-      <c r="B82" s="9">
+      <c r="B90" s="9">
         <v>0.83187169999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="10">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="10">
         <v>42.059730000000002</v>
       </c>
-      <c r="B83" s="9">
+      <c r="B91" s="9">
         <v>0.57295079999999998</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="10">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="10">
         <v>42.059730000000002</v>
       </c>
-      <c r="B84" s="9">
+      <c r="B92" s="9">
         <v>1.7377849999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="10">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="10">
         <v>42.059730000000002</v>
       </c>
-      <c r="B85" s="9">
+      <c r="B93" s="9">
         <v>1.593799</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="10">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="10">
         <v>42.059730000000002</v>
       </c>
-      <c r="B86" s="9">
+      <c r="B94" s="9">
         <v>1.0861190000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="10">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="10">
         <v>42.059730000000002</v>
       </c>
-      <c r="B87" s="9">
+      <c r="B95" s="9">
         <v>0.96393479999999998</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="10">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="10">
         <v>42.059730000000002</v>
       </c>
-      <c r="B88" s="9">
+      <c r="B96" s="9">
         <v>1.6751320000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="10">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="10">
         <v>42.059730000000002</v>
       </c>
-      <c r="B89" s="9">
+      <c r="B97" s="9">
         <v>3.156685</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed 41 deg 48 hr
</commit_message>
<xml_diff>
--- a/data-raw/growth_rates_summary_wip.xlsx
+++ b/data-raw/growth_rates_summary_wip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sveta\Documents\B Lab\cross-tolerance\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D059B9-5DF1-4584-926B-0D0B68AE5135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1B30DEC-9F0B-4AF4-8A2C-C2B355B787DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{311CE9AC-D601-4DF3-8159-B4D668D6C29C}"/>
   </bookViews>
@@ -171,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -188,7 +188,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -604,10 +603,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33C40890-5FB8-4C42-A3AD-60610C49A445}">
-  <dimension ref="A1:D97"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="D83" sqref="D83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +621,7 @@
       <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="15"/>
+      <c r="D1" s="14"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
@@ -817,7 +816,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+      <c r="A26" s="16">
         <v>30.255669999999999</v>
       </c>
       <c r="B26">
@@ -825,7 +824,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+      <c r="A27" s="16">
         <v>30.255669999999999</v>
       </c>
       <c r="B27">
@@ -833,7 +832,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="17">
+      <c r="A28" s="16">
         <v>30.255669999999999</v>
       </c>
       <c r="B28">
@@ -841,7 +840,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="17">
+      <c r="A29" s="16">
         <v>30.255669999999999</v>
       </c>
       <c r="B29">
@@ -849,7 +848,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="17">
+      <c r="A30" s="16">
         <v>30.255669999999999</v>
       </c>
       <c r="B30">
@@ -857,7 +856,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" s="17">
+      <c r="A31" s="16">
         <v>30.255669999999999</v>
       </c>
       <c r="B31">
@@ -865,7 +864,7 @@
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="17">
+      <c r="A32" s="16">
         <v>30.255669999999999</v>
       </c>
       <c r="B32">
@@ -873,7 +872,7 @@
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17">
+      <c r="A33" s="16">
         <v>30.255669999999999</v>
       </c>
       <c r="B33">
@@ -1265,130 +1264,66 @@
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="8">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B82" s="6">
-        <v>2.772583</v>
+      <c r="A82" s="9">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B82" s="8">
+        <v>0.83187169999999999</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="8">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B83" s="6">
-        <v>2.6771850000000001</v>
+      <c r="A83" s="9">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B83" s="8">
+        <v>0.57295079999999998</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="8">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B84" s="6">
-        <v>2.5681379999999998</v>
+      <c r="A84" s="9">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B84" s="8">
+        <v>1.7377849999999999</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="8">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B85" s="6">
-        <v>2.593191</v>
+      <c r="A85" s="9">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B85" s="8">
+        <v>1.593799</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="8">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B86" s="6">
-        <v>1.9705459999999999</v>
+      <c r="A86" s="9">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B86" s="8">
+        <v>1.0861190000000001</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="8">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B87" s="6">
-        <v>2.7541199999999999</v>
+      <c r="A87" s="9">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B87" s="8">
+        <v>0.96393479999999998</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="8">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B88" s="6">
-        <v>2.6078480000000002</v>
+      <c r="A88" s="9">
+        <v>42.059730000000002</v>
+      </c>
+      <c r="B88" s="8">
+        <v>1.6751320000000001</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="8">
-        <v>40.980829999999997</v>
-      </c>
-      <c r="B89" s="6">
-        <v>2.4336829999999998</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="10">
+      <c r="A89" s="9">
         <v>42.059730000000002</v>
       </c>
-      <c r="B90" s="9">
-        <v>0.83187169999999999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="10">
-        <v>42.059730000000002</v>
-      </c>
-      <c r="B91" s="9">
-        <v>0.57295079999999998</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="10">
-        <v>42.059730000000002</v>
-      </c>
-      <c r="B92" s="9">
-        <v>1.7377849999999999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="10">
-        <v>42.059730000000002</v>
-      </c>
-      <c r="B93" s="9">
-        <v>1.593799</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="10">
-        <v>42.059730000000002</v>
-      </c>
-      <c r="B94" s="9">
-        <v>1.0861190000000001</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="10">
-        <v>42.059730000000002</v>
-      </c>
-      <c r="B95" s="9">
-        <v>0.96393479999999998</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="10">
-        <v>42.059730000000002</v>
-      </c>
-      <c r="B96" s="9">
-        <v>1.6751320000000001</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="10">
-        <v>42.059730000000002</v>
-      </c>
-      <c r="B97" s="9">
+      <c r="B89" s="8">
         <v>3.156685</v>
       </c>
     </row>
@@ -1417,581 +1352,581 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>18</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>0.1003318</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>18</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>9.9472599999999994E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>18</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>9.9491599999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>18</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>9.8961099999999996E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>18</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>0.10189860000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>18</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>9.7996799999999995E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>18</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>9.76442E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>18</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>0.10099859999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>25.367419999999999</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>6.9786530000000004</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>7.1318700000000002</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <v>5.4270839999999998</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <v>7.1399920000000003</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>7.0237829999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>7.2581819999999997</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>7.1565450000000004</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
+      <c r="A17" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>7.0355239999999997</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B18" s="12">
+      <c r="A18" s="12">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B18" s="11">
         <v>8.8879839999999994</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B19" s="12">
+      <c r="A19" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B19" s="11">
         <v>9.1432889999999993</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B20" s="12">
+      <c r="A20" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B20" s="11">
         <v>8.8955749999999991</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B21" s="12">
+      <c r="A21" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B21" s="11">
         <v>9.0471590000000006</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B22" s="12">
+      <c r="A22" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B22" s="11">
         <v>9.0021679999999993</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B23" s="12">
+      <c r="A23" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B23" s="11">
         <v>8.9892319999999994</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B24" s="12">
+      <c r="A24" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B24" s="11">
         <v>10.67995</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B25" s="12">
+      <c r="A25" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B25" s="11">
         <v>8.9228000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B26" s="12">
+      <c r="A26" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B26" s="11">
         <v>8.9139230000000005</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B27" s="12">
+      <c r="A27" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B27" s="11">
         <v>9.0081030000000002</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B28" s="12">
+      <c r="A28" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B28" s="11">
         <v>8.7893570000000008</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B29" s="12">
+      <c r="A29" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B29" s="11">
         <v>8.7185349999999993</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13">
+      <c r="A30" s="12">
         <v>37.310420000000001</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="11">
         <v>8.0510959999999994</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14">
+      <c r="A31" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="11">
         <v>8.1196149999999996</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14">
+      <c r="A32" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="11">
         <v>11.442589999999999</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14">
+      <c r="A33" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="11">
         <v>10.72757</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14">
+      <c r="A34" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="11">
         <v>10.68343</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14">
+      <c r="A35" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="11">
         <v>11.225</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14">
+      <c r="A36" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="11">
         <v>10.61753</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14">
+      <c r="A37" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="11">
         <v>8.0467929999999992</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14">
+      <c r="A38" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="11">
         <v>10.187290000000001</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14">
+      <c r="A39" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39" s="11">
         <v>7.463965</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="14">
+      <c r="A40" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="11">
         <v>9.7239989999999992</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="14">
+      <c r="A41" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="11">
         <v>5.4158989999999996</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="14">
+      <c r="A42" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="11">
         <v>10.54608</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="14">
+      <c r="A43" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B43" s="11">
         <v>7.5910469999999997</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="14">
+      <c r="A44" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="11">
         <v>10.436120000000001</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="14">
+      <c r="A45" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45" s="11">
         <v>10.63997</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="14">
+      <c r="A46" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B46" s="12">
+      <c r="B46" s="11">
         <v>6.7881</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14">
+      <c r="A47" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B47" s="12">
+      <c r="B47" s="11">
         <v>6.3737240000000002</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="14">
+      <c r="A48" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B48" s="12">
+      <c r="B48" s="11">
         <v>3.1252529999999998</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14">
+      <c r="A49" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B49" s="12">
+      <c r="B49" s="11">
         <v>3.9723419999999998</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="14">
+      <c r="A50" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B50" s="12">
+      <c r="B50" s="11">
         <v>3.2859699999999998</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="14">
+      <c r="A51" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B51" s="12">
+      <c r="B51" s="11">
         <v>6.0659299999999998</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="14">
+      <c r="A52" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B52" s="12">
+      <c r="B52" s="11">
         <v>7.9045569999999996</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="14">
+      <c r="A53" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B53" s="12">
+      <c r="B53" s="11">
         <v>8.5736969999999992</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="13">
+      <c r="A54" s="12">
         <v>41.180900000000001</v>
       </c>
-      <c r="B54" s="12">
+      <c r="B54" s="11">
         <v>1.248718</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="14">
+      <c r="A55" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B55" s="12">
+      <c r="B55" s="11">
         <v>8.7624300000000002</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="14">
+      <c r="A56" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B56" s="12">
+      <c r="B56" s="11">
         <v>0.76345470000000004</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="14">
+      <c r="A57" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B57" s="12">
+      <c r="B57" s="11">
         <v>0.5987903</v>
       </c>
-      <c r="D57" s="15">
+      <c r="D57" s="14">
         <v>45107</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="14">
+      <c r="A58" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B58" s="12">
+      <c r="B58" s="11">
         <v>0.4896916</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="14">
+      <c r="A59" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B59" s="12">
+      <c r="B59" s="11">
         <v>0.48276409999999997</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="14">
+      <c r="A60" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B60" s="12">
+      <c r="B60" s="11">
         <v>0.48143750000000002</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="14">
+      <c r="A61" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B61" s="12">
+      <c r="B61" s="11">
         <v>0.50883769999999995</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="14">
+      <c r="A62" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B62" s="12">
+      <c r="B62" s="11">
         <v>0.86194800000000005</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="14">
+      <c r="A63" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B63" s="12">
+      <c r="B63" s="11">
         <v>1.178188</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="14">
+      <c r="A64" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B64" s="12">
+      <c r="B64" s="11">
         <v>1.075391</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="14">
+      <c r="A65" s="13">
         <v>41.180900000000001</v>
       </c>
-      <c r="B65" s="12">
+      <c r="B65" s="11">
         <v>1.583267</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="16">
+      <c r="A66" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B66" s="12">
+      <c r="B66" s="11">
         <v>0.83187169999999999</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="16">
+      <c r="A67" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B67" s="12">
+      <c r="B67" s="11">
         <v>0.57295079999999998</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="16">
+      <c r="A68" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B68" s="12">
+      <c r="B68" s="11">
         <v>1.7377849999999999</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="16">
+      <c r="A69" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B69" s="12">
+      <c r="B69" s="11">
         <v>1.593799</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="16">
+      <c r="A70" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B70" s="12">
+      <c r="B70" s="11">
         <v>1.0861190000000001</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="16">
+      <c r="A71" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B71" s="12">
+      <c r="B71" s="11">
         <v>0.96393479999999998</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="16">
+      <c r="A72" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B72" s="12">
+      <c r="B72" s="11">
         <v>1.6751320000000001</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="16">
+      <c r="A73" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B73" s="12">
+      <c r="B73" s="11">
         <v>3.156685</v>
       </c>
     </row>
@@ -2019,546 +1954,546 @@
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11">
+      <c r="A2" s="10">
         <v>18</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="11">
         <v>0.1003318</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="11">
+      <c r="A3" s="10">
         <v>18</v>
       </c>
-      <c r="B3" s="12">
+      <c r="B3" s="11">
         <v>9.9472599999999994E-2</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11">
+      <c r="A4" s="10">
         <v>18</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4" s="11">
         <v>9.9491599999999999E-2</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11">
+      <c r="A5" s="10">
         <v>18</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5" s="11">
         <v>9.8961099999999996E-2</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="11">
+      <c r="A6" s="10">
         <v>18</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6" s="11">
         <v>0.10189860000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="11">
+      <c r="A7" s="10">
         <v>18</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7" s="11">
         <v>9.7996799999999995E-2</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11">
+      <c r="A8" s="10">
         <v>18</v>
       </c>
-      <c r="B8" s="12">
+      <c r="B8" s="11">
         <v>9.76442E-2</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11">
+      <c r="A9" s="10">
         <v>18</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9" s="11">
         <v>0.10099859999999999</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13">
+      <c r="A10" s="12">
         <v>25.367419999999999</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10" s="11">
         <v>6.9786530000000004</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14">
+      <c r="A11" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B11" s="12">
+      <c r="B11" s="11">
         <v>7.1318700000000002</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="14">
+      <c r="A12" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B12" s="12">
+      <c r="B12" s="11">
         <v>5.4270839999999998</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="14">
+      <c r="A13" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B13" s="12">
+      <c r="B13" s="11">
         <v>7.1399920000000003</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="14">
+      <c r="A14" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B14" s="12">
+      <c r="B14" s="11">
         <v>7.0237829999999999</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="14">
+      <c r="A15" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B15" s="12">
+      <c r="B15" s="11">
         <v>7.2581819999999997</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="14">
+      <c r="A16" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>7.1565450000000004</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="14">
+      <c r="A17" s="13">
         <v>25.367419999999999</v>
       </c>
-      <c r="B17" s="12">
+      <c r="B17" s="11">
         <v>7.0355239999999997</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="13">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B18" s="12">
+      <c r="A18" s="12">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B18" s="11">
         <v>8.8879839999999994</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B19" s="12">
+      <c r="A19" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B19" s="11">
         <v>9.1432889999999993</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B20" s="12">
+      <c r="A20" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B20" s="11">
         <v>8.8955749999999991</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B21" s="12">
+      <c r="A21" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B21" s="11">
         <v>9.0471590000000006</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B22" s="12">
+      <c r="A22" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B22" s="11">
         <v>9.0021679999999993</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B23" s="12">
+      <c r="A23" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B23" s="11">
         <v>8.9892319999999994</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B24" s="12">
+      <c r="A24" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B24" s="11">
         <v>10.67995</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B25" s="12">
+      <c r="A25" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B25" s="11">
         <v>8.9228000000000005</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B26" s="12">
+      <c r="A26" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B26" s="11">
         <v>8.9139230000000005</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B27" s="12">
+      <c r="A27" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B27" s="11">
         <v>9.0081030000000002</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B28" s="12">
+      <c r="A28" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B28" s="11">
         <v>8.7893570000000008</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="14">
-        <v>34.135959999999997</v>
-      </c>
-      <c r="B29" s="12">
+      <c r="A29" s="13">
+        <v>34.135959999999997</v>
+      </c>
+      <c r="B29" s="11">
         <v>8.7185349999999993</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="13">
+      <c r="A30" s="12">
         <v>37.310420000000001</v>
       </c>
-      <c r="B30" s="12">
+      <c r="B30" s="11">
         <v>8.0510959999999994</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="14">
+      <c r="A31" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B31" s="12">
+      <c r="B31" s="11">
         <v>8.1196149999999996</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="14">
+      <c r="A32" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="11">
         <v>11.442589999999999</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="14">
+      <c r="A33" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B33" s="12">
+      <c r="B33" s="11">
         <v>10.72757</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="14">
+      <c r="A34" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B34" s="12">
+      <c r="B34" s="11">
         <v>10.68343</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="14">
+      <c r="A35" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B35" s="12">
+      <c r="B35" s="11">
         <v>11.225</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="14">
+      <c r="A36" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B36" s="12">
+      <c r="B36" s="11">
         <v>10.61753</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="14">
+      <c r="A37" s="13">
         <v>37.310420000000001</v>
       </c>
-      <c r="B37" s="12">
+      <c r="B37" s="11">
         <v>8.0467929999999992</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="14">
+      <c r="A38" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B38" s="12">
+      <c r="B38" s="11">
         <v>10.187290000000001</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="14">
+      <c r="A39" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B39" s="12">
+      <c r="B39" s="11">
         <v>7.463965</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="14">
+      <c r="A40" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B40" s="12">
+      <c r="B40" s="11">
         <v>9.7239989999999992</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="14">
+      <c r="A41" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B41" s="12">
+      <c r="B41" s="11">
         <v>5.4158989999999996</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="14">
+      <c r="A42" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B42" s="12">
+      <c r="B42" s="11">
         <v>10.54608</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="14">
+      <c r="A43" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B43" s="12">
+      <c r="B43" s="11">
         <v>7.5910469999999997</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="14">
+      <c r="A44" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B44" s="12">
+      <c r="B44" s="11">
         <v>10.436120000000001</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="14">
+      <c r="A45" s="13">
         <v>40.116849999999999</v>
       </c>
-      <c r="B45" s="12">
+      <c r="B45" s="11">
         <v>10.63997</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="14">
+      <c r="A46" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B46" s="12">
+      <c r="B46" s="11">
         <v>6.7881</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="14">
+      <c r="A47" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B47" s="12">
+      <c r="B47" s="11">
         <v>6.3737240000000002</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="14">
+      <c r="A48" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B48" s="12">
+      <c r="B48" s="11">
         <v>3.1252529999999998</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="14">
+      <c r="A49" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B49" s="12">
+      <c r="B49" s="11">
         <v>3.9723419999999998</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="14">
+      <c r="A50" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B50" s="12">
+      <c r="B50" s="11">
         <v>3.2859699999999998</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="14">
+      <c r="A51" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B51" s="12">
+      <c r="B51" s="11">
         <v>6.0659299999999998</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="14">
+      <c r="A52" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B52" s="12">
+      <c r="B52" s="11">
         <v>7.9045569999999996</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="14">
+      <c r="A53" s="13">
         <v>40.535420000000002</v>
       </c>
-      <c r="B53" s="12">
+      <c r="B53" s="11">
         <v>8.5736969999999992</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="16">
+      <c r="A54" s="15">
         <v>40.980829999999997</v>
       </c>
-      <c r="B54" s="12">
+      <c r="B54" s="11">
         <v>2.772583</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="16">
+      <c r="A55" s="15">
         <v>40.980829999999997</v>
       </c>
-      <c r="B55" s="12">
+      <c r="B55" s="11">
         <v>2.6771850000000001</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="16">
+      <c r="A56" s="15">
         <v>40.980829999999997</v>
       </c>
-      <c r="B56" s="12">
+      <c r="B56" s="11">
         <v>2.5681379999999998</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="16">
+      <c r="A57" s="15">
         <v>40.980829999999997</v>
       </c>
-      <c r="B57" s="12">
+      <c r="B57" s="11">
         <v>2.593191</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="16">
+      <c r="A58" s="15">
         <v>40.980829999999997</v>
       </c>
-      <c r="B58" s="12">
+      <c r="B58" s="11">
         <v>1.9705459999999999</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="16">
+      <c r="A59" s="15">
         <v>40.980829999999997</v>
       </c>
-      <c r="B59" s="12">
+      <c r="B59" s="11">
         <v>2.7541199999999999</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="16">
+      <c r="A60" s="15">
         <v>40.980829999999997</v>
       </c>
-      <c r="B60" s="12">
+      <c r="B60" s="11">
         <v>2.6078480000000002</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="16">
+      <c r="A61" s="15">
         <v>40.980829999999997</v>
       </c>
-      <c r="B61" s="12">
+      <c r="B61" s="11">
         <v>2.4336829999999998</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="16">
+      <c r="A62" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B62" s="12">
+      <c r="B62" s="11">
         <v>0.83187169999999999</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="16">
+      <c r="A63" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B63" s="12">
+      <c r="B63" s="11">
         <v>0.57295079999999998</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="16">
+      <c r="A64" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B64" s="12">
+      <c r="B64" s="11">
         <v>1.7377849999999999</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="16">
+      <c r="A65" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B65" s="12">
+      <c r="B65" s="11">
         <v>1.593799</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="16">
+      <c r="A66" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B66" s="12">
+      <c r="B66" s="11">
         <v>1.0861190000000001</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="16">
+      <c r="A67" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B67" s="12">
+      <c r="B67" s="11">
         <v>0.96393479999999998</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="16">
+      <c r="A68" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B68" s="12">
+      <c r="B68" s="11">
         <v>1.6751320000000001</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="16">
+      <c r="A69" s="15">
         <v>42.059730000000002</v>
       </c>
-      <c r="B69" s="12">
+      <c r="B69" s="11">
         <v>3.156685</v>
       </c>
     </row>

</xml_diff>